<commit_message>
order medication + report generation + delete presec
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/AL Hilal Group.xlsx
+++ b/Insurance/insurance_templates/AL Hilal Group.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noor/ALGAEH/DEV/algaeh-monorepo/Insurance/insurance_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\algaeh-monorepo\Insurance\insurance_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B37A2054-8F87-B540-AA53-39979DB31AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D55FF094-03CB-4BD1-A517-6BD778FAE6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="19" uniqueCount="19">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="44" uniqueCount="22">
   <si>
     <t>Patient Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Net Amt</t>
   </si>
   <si>
-    <t>NAME OF HOSPITAL :- DR.ABDULLA KAMAL CLINIC</t>
-  </si>
-  <si>
     <t>Policy No.</t>
   </si>
   <si>
@@ -91,7 +88,19 @@
     <t>VAT Rate</t>
   </si>
   <si>
-    <t>MEDICAL CLAIMS STATEMENT FOR THE MONTH OF :- AUGUST - 2020</t>
+    <t>DR.ABDULLA KAMAL CLINIC</t>
+  </si>
+  <si>
+    <t>MEDICAL CLAIMS STATEMENT FOR THE MONTH OF :-</t>
+  </si>
+  <si>
+    <t>NAME OF HOSPITAL:-</t>
+  </si>
+  <si>
+    <t>From:  #FDATE</t>
+  </si>
+  <si>
+    <t>To:  #TDATE</t>
   </si>
 </sst>
 </file>
@@ -101,27 +110,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -131,58 +122,42 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="36"/>
-      <name val="Monotype Corsiva"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="10"/>
+      <sz val="12"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <name val="Bookman Old Style"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="24"/>
-      <name val="Arial Rounded MT Bold"/>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <start/>
       <end/>
@@ -191,95 +166,54 @@
       <diagonal/>
     </border>
     <border>
-      <start style="medium">
-        <color indexed="64"/>
+      <start style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </start>
-      <end/>
-      <top style="medium">
-        <color indexed="64"/>
+      <end style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </end>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start style="medium">
-        <color indexed="64"/>
-      </start>
-      <end style="medium">
-        <color indexed="64"/>
-      </end>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <start style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.499984740745262"/>
       </start>
       <end/>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </end>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <start/>
       <end/>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start style="thin">
-        <color indexed="64"/>
-      </start>
-      <end style="thin">
-        <color indexed="64"/>
-      </end>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start/>
-      <end style="thin">
-        <color indexed="64"/>
-      </end>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start/>
-      <end style="medium">
-        <color indexed="64"/>
-      </end>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -287,53 +221,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,23 +351,23 @@
 <xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1422400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1190789</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1162050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6370" name="Picture 1" descr="Logo.png">
+        <xdr:cNvPr id="4" name="Picture 3" descr="Logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43095A2D-4C02-1B42-9D01-09C905B93287}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{244BBDAD-5274-4221-803F-08072733602E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -463,8 +390,87 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="876300" y="177800"/>
-          <a:ext cx="6705600" cy="1625600"/>
+          <a:off x="190501" y="123826"/>
+          <a:ext cx="2248063" cy="1038224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800%"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1040692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7971C7D3-4A36-4DF7-AD37-F0551A04EDC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="190501" y="123825"/>
+          <a:ext cx="3429000" cy="916867"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -821,136 +827,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="49.5" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="83" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="42" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" customWidth="1"/>
-    <col min="23" max="23" width="34.1640625" customWidth="1"/>
-    <col min="24" max="24" width="37.1640625" customWidth="1"/>
-    <col min="25" max="25" width="38.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.28515625" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="F1">
+    <row r="1" spans="1:17" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="25" x14ac:dyDescent="0.25">
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="48" x14ac:dyDescent="0.6">
-      <c r="E4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.2">
-      <c r="F7" s="3"/>
-    </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="13" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:17" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="I4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="14" t="s">
+      <c r="K4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="N4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="N14" s="20" t="s">
+      <c r="O4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="P14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q14" s="22" t="s">
+      <c r="Q4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:Q3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup scale="24" fitToHeight="2" orientation="landscape"/>
@@ -964,16 +996,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:Q3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -983,9 +1168,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Updated Insurance Statement Excel
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/AL Hilal Group.xlsx
+++ b/Insurance/insurance_templates/AL Hilal Group.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\algaeh-monorepo\Insurance\insurance_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D55FF094-03CB-4BD1-A517-6BD778FAE6A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{346B630F-C626-4E46-BD53-134A96250C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <start/>
       <end/>
@@ -217,11 +217,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </start>
+      <end style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </end>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -229,37 +244,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -830,145 +864,146 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.28515625" customWidth="1"/>
-    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.28515625" style="15" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
     </row>
-    <row r="2" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="7"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
     </row>
     <row r="4" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1025,134 +1060,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="7"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:Q3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:Q2"/>
-    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>